<commit_message>
Adicionando rodadas 35 a 38 no arquivo com esquema tatico 4-4-2
</commit_message>
<xml_diff>
--- a/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos.xlsx
+++ b/analises_dos_dados_preliminares/4-4-2 -----Times mais caros por rodada X Times Escolhidos Pelo algoritmos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpcrj\OneDrive\Área de Trabalho\Faculdade\TCC_code\sportsAnalytics\analises_dos_dados_preliminares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93930C5F-8876-4DAB-8845-FA42C407AD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB9A47D-25FD-4C66-9E33-DD6EB5444ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="15" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="15" xr2:uid="{FCE826C4-9F25-4A22-BADC-C872D1D1AAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="rodada 19" sheetId="20" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="52">
   <si>
     <t>Anderson Hernanes de Carvalho Andrade Lima</t>
   </si>
@@ -178,12 +178,6 @@
     <t>Pedro Henrique Ribeiro Gonçalves</t>
   </si>
   <si>
-    <t>Ev</t>
-  </si>
-  <si>
-    <t>Giorgian</t>
-  </si>
-  <si>
     <t>Tiago dos Santos Alves</t>
   </si>
   <si>
@@ -209,6 +203,12 @@
   </si>
   <si>
     <t>FALTA UM JOGADOR NA CONSULTA</t>
+  </si>
+  <si>
+    <t>Artur Victor Guimarães</t>
+  </si>
+  <si>
+    <t>Marcos Roberto da Silva Barbosa</t>
   </si>
 </sst>
 </file>
@@ -287,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -333,6 +333,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,7 +915,7 @@
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2">
         <v>72018</v>
@@ -927,7 +930,7 @@
         <v>5.3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G4" s="9">
         <v>72018</v>
@@ -1694,7 +1697,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -1709,7 +1712,7 @@
         <v>4.55</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9">
         <v>41929</v>
@@ -2282,7 +2285,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -2297,7 +2300,7 @@
         <v>4.54</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9">
         <v>41929</v>
@@ -2866,7 +2869,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -2881,7 +2884,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3">
         <v>41929</v>
@@ -3390,7 +3393,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -3405,7 +3408,7 @@
         <v>4.63</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3">
         <v>41929</v>
@@ -4309,7 +4312,7 @@
         <v>10.06</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3">
         <v>80393</v>
@@ -4402,7 +4405,7 @@
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
         <v>80393</v>
@@ -4813,7 +4816,7 @@
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>80393</v>
@@ -4838,7 +4841,7 @@
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
@@ -4948,10 +4951,597 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0BEAF9-D8E7-4D4A-BBF1-8174DFBBF3FC}">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J13"/>
+      <selection activeCell="A7" sqref="A7:XFD10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="16.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="22" style="9" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="9"/>
+    <col min="11" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2">
+        <v>86757</v>
+      </c>
+      <c r="C2" s="2">
+        <v>17.03</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7.09</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="9">
+        <v>86757</v>
+      </c>
+      <c r="H2" s="9">
+        <v>17.03</v>
+      </c>
+      <c r="I2" s="9">
+        <v>2</v>
+      </c>
+      <c r="J2" s="9">
+        <v>7.09</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2">
+        <v>91607</v>
+      </c>
+      <c r="C3" s="2">
+        <v>14.3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8.6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="9">
+        <v>91607</v>
+      </c>
+      <c r="H3" s="9">
+        <v>14.3</v>
+      </c>
+      <c r="I3" s="9">
+        <v>8.6</v>
+      </c>
+      <c r="J3" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+    </row>
+    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2">
+        <v>82453</v>
+      </c>
+      <c r="C4" s="2">
+        <v>17.8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.08</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9">
+        <v>82453</v>
+      </c>
+      <c r="H4" s="9">
+        <v>17.8</v>
+      </c>
+      <c r="I4" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="J4" s="9">
+        <v>7.08</v>
+      </c>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+    </row>
+    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2">
+        <v>78850</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15.83</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9">
+        <v>42500</v>
+      </c>
+      <c r="H5" s="9">
+        <v>14.3</v>
+      </c>
+      <c r="I5" s="9">
+        <v>12.4</v>
+      </c>
+      <c r="J5" s="9">
+        <v>5.24</v>
+      </c>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+    </row>
+    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42500</v>
+      </c>
+      <c r="C6" s="2">
+        <v>14.3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12.4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9">
+        <v>78850</v>
+      </c>
+      <c r="H6" s="9">
+        <v>15.83</v>
+      </c>
+      <c r="I6" s="9">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J6" s="9">
+        <v>5.95</v>
+      </c>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+    </row>
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>87863</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17.77</v>
+      </c>
+      <c r="D7" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="9">
+        <v>85465</v>
+      </c>
+      <c r="H7" s="9">
+        <v>9.66</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="9">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+    </row>
+    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>98706</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12.18</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="9">
+        <v>87863</v>
+      </c>
+      <c r="H8" s="9">
+        <v>17.77</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="J8" s="9">
+        <v>10.029999999999999</v>
+      </c>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+    </row>
+    <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2">
+        <v>85465</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9.66</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="9">
+        <v>92496</v>
+      </c>
+      <c r="H9" s="9">
+        <v>7.7</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="J9" s="9">
+        <v>4.08</v>
+      </c>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+    </row>
+    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="2">
+        <v>92496</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.08</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="9">
+        <v>98706</v>
+      </c>
+      <c r="H10" s="9">
+        <v>12.18</v>
+      </c>
+      <c r="I10" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="J10" s="9">
+        <v>5.18</v>
+      </c>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+    </row>
+    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2">
+        <v>70800</v>
+      </c>
+      <c r="C11" s="2">
+        <v>12.59</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="9">
+        <v>70800</v>
+      </c>
+      <c r="H11" s="9">
+        <v>12.59</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+    </row>
+    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>80853</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12.4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5.39</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9">
+        <v>52253</v>
+      </c>
+      <c r="H12" s="9">
+        <v>12.07</v>
+      </c>
+      <c r="I12" s="9">
+        <v>3.3</v>
+      </c>
+      <c r="J12" s="9">
+        <v>4.55</v>
+      </c>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+    </row>
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2">
+        <v>52253</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12.07</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.55</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9">
+        <v>80853</v>
+      </c>
+      <c r="H13" s="9">
+        <v>12.4</v>
+      </c>
+      <c r="I13" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="J13" s="9">
+        <v>5.39</v>
+      </c>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+    </row>
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5">
+        <f>SUM(C2:C13)</f>
+        <v>163.63</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="9">
+        <f>SUM(H2:H13)</f>
+        <v>163.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+      <c r="D16" s="8"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E01322-0607-4F4D-8EF5-9D4D083FB770}">
+  <dimension ref="A1:AD16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5012,270 +5602,457 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="9"/>
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2">
+        <v>83257</v>
+      </c>
+      <c r="C2" s="2">
+        <v>23.7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>23.6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9.85</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>83257</v>
+      </c>
+      <c r="H2" s="9">
+        <v>23.7</v>
+      </c>
+      <c r="I2" s="9">
+        <v>23.6</v>
+      </c>
+      <c r="J2" s="9">
+        <v>9.85</v>
+      </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2">
+        <v>86757</v>
+      </c>
+      <c r="C3" s="2">
+        <v>17.88</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.8</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.05</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="9">
+        <v>86757</v>
+      </c>
+      <c r="H3" s="9">
+        <v>17.88</v>
+      </c>
+      <c r="I3" s="9">
+        <v>5.8</v>
+      </c>
+      <c r="J3" s="9">
+        <v>7.05</v>
+      </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="9"/>
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2">
+        <v>82453</v>
+      </c>
+      <c r="C4" s="2">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7.02</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9">
+        <v>82453</v>
+      </c>
+      <c r="H4" s="9">
+        <v>16.739999999999998</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5</v>
+      </c>
+      <c r="J4" s="9">
+        <v>7.02</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2">
+        <v>78850</v>
+      </c>
+      <c r="C5" s="2">
+        <v>14.75</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.81</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9">
+        <v>42500</v>
+      </c>
+      <c r="H5" s="9">
+        <v>12.49</v>
+      </c>
+      <c r="I5" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="J5" s="9">
+        <v>5.03</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42500</v>
+      </c>
+      <c r="C6" s="2">
+        <v>12.49</v>
+      </c>
+      <c r="D6" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.03</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9">
+        <v>78850</v>
+      </c>
+      <c r="H6" s="9">
+        <v>14.75</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>5.81</v>
+      </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>87863</v>
+      </c>
+      <c r="C7" s="2">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="D7" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10.26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="9">
+        <v>80393</v>
+      </c>
+      <c r="H7" s="9">
+        <v>7.37</v>
+      </c>
+      <c r="I7" s="9">
+        <v>6.2</v>
+      </c>
+      <c r="J7" s="9">
+        <v>2.39</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>98706</v>
+      </c>
+      <c r="C8" s="2">
+        <v>12.03</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="9">
+        <v>85465</v>
+      </c>
+      <c r="H8" s="9">
+        <v>9.15</v>
+      </c>
+      <c r="I8" s="9">
+        <v>-2.9</v>
+      </c>
+      <c r="J8" s="9">
+        <v>3.93</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2">
+        <v>85465</v>
+      </c>
+      <c r="C9" s="2">
+        <v>9.15</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-2.9</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.93</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9">
+        <v>87863</v>
+      </c>
+      <c r="H9" s="9">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="I9" s="9">
+        <v>14.6</v>
+      </c>
+      <c r="J9" s="9">
+        <v>10.26</v>
+      </c>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2">
+        <v>80393</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.37</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.39</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="9">
+        <v>98706</v>
+      </c>
+      <c r="H10" s="9">
+        <v>12.03</v>
+      </c>
+      <c r="I10" s="9">
+        <v>3.4</v>
+      </c>
+      <c r="J10" s="9">
+        <v>5.1100000000000003</v>
+      </c>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2">
+        <v>70800</v>
+      </c>
+      <c r="C11" s="2">
+        <v>13.71</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5.97</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.68</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="9">
+        <v>70800</v>
+      </c>
+      <c r="H11" s="9">
+        <v>13.71</v>
+      </c>
+      <c r="I11" s="9">
+        <v>5.97</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.68</v>
+      </c>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>80853</v>
+      </c>
+      <c r="C12" s="2">
+        <v>13.54</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5.46</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9">
+        <v>52253</v>
+      </c>
+      <c r="H12" s="9">
+        <v>11.64</v>
+      </c>
+      <c r="I12" s="9">
+        <v>-0.1</v>
+      </c>
+      <c r="J12" s="9">
+        <v>4.38</v>
+      </c>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2">
+        <v>52253</v>
+      </c>
+      <c r="C13" s="2">
+        <v>11.64</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-0.1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.38</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9">
+        <v>80853</v>
+      </c>
+      <c r="H13" s="9">
+        <v>13.54</v>
+      </c>
+      <c r="I13" s="9">
+        <v>6.7</v>
+      </c>
+      <c r="J13" s="9">
+        <v>5.46</v>
+      </c>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
     </row>
-    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="7"/>
-    </row>
+    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C13)</f>
-        <v>0</v>
+        <v>172.01</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="9">
         <f>SUM(H2:H13)</f>
-        <v>0</v>
+        <v>172.01000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5283,12 +6060,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E01322-0607-4F4D-8EF5-9D4D083FB770}">
-  <dimension ref="A1:AD28"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FC2FBA-017B-4C34-B19F-488BCA852EC5}">
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5299,9 +6076,9 @@
     <col min="4" max="5" width="16.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="36.28515625" style="7" customWidth="1"/>
     <col min="7" max="7" width="22" style="9" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="29.42578125" style="9" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="9"/>
+    <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -5326,15 +6103,16 @@
       <c r="G1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="11" t="s">
         <v>26</v>
       </c>
+      <c r="K1" s="11"/>
       <c r="AA1" s="4" t="s">
         <v>12</v>
       </c>
@@ -5349,180 +6127,432 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="9"/>
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2">
+        <v>83257</v>
+      </c>
+      <c r="C2" s="2">
+        <v>21.94</v>
+      </c>
+      <c r="D2" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>83257</v>
+      </c>
+      <c r="H2" s="9">
+        <v>21.94</v>
+      </c>
+      <c r="I2" s="9">
+        <v>13.8</v>
+      </c>
+      <c r="J2" s="9">
+        <v>10</v>
+      </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="9"/>
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2">
+        <v>86757</v>
+      </c>
+      <c r="C3" s="2">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5.3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.99</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="9">
+        <v>86757</v>
+      </c>
+      <c r="H3" s="9">
+        <v>17.489999999999998</v>
+      </c>
+      <c r="I3" s="9">
+        <v>5.3</v>
+      </c>
+      <c r="J3" s="9">
+        <v>6.99</v>
+      </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="9"/>
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2">
+        <v>82453</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14.38</v>
+      </c>
+      <c r="D4" s="2">
+        <v>-7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6.62</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9">
+        <v>82453</v>
+      </c>
+      <c r="H4" s="9">
+        <v>14.38</v>
+      </c>
+      <c r="I4" s="9">
+        <v>-7</v>
+      </c>
+      <c r="J4" s="9">
+        <v>6.62</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2">
+        <v>78850</v>
+      </c>
+      <c r="C5" s="2">
+        <v>14.37</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.67</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9">
+        <v>42500</v>
+      </c>
+      <c r="H5" s="9">
+        <v>13.37</v>
+      </c>
+      <c r="I5" s="9">
+        <v>6.8</v>
+      </c>
+      <c r="J5" s="9">
+        <v>5.0999999999999996</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42500</v>
+      </c>
+      <c r="C6" s="2">
+        <v>13.37</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9">
+        <v>78850</v>
+      </c>
+      <c r="H6" s="9">
+        <v>14.37</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="J6" s="9">
+        <v>5.67</v>
+      </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>87863</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20.21</v>
+      </c>
+      <c r="D7" s="2">
+        <v>22.4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10.84</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>51772</v>
+      </c>
+      <c r="H7" s="9">
+        <v>12.28</v>
+      </c>
+      <c r="I7" s="9">
+        <v>5.6</v>
+      </c>
+      <c r="J7" s="9">
+        <v>3.53</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2">
+        <v>92496</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8.24</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.08</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="9">
+        <v>80393</v>
+      </c>
+      <c r="H8" s="9">
+        <v>6.62</v>
+      </c>
+      <c r="I8" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="J8" s="9">
+        <v>2.38</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>51772</v>
+      </c>
+      <c r="C9" s="2">
+        <v>12.28</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.53</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9">
+        <v>87863</v>
+      </c>
+      <c r="H9" s="9">
+        <v>20.21</v>
+      </c>
+      <c r="I9" s="9">
+        <v>22.4</v>
+      </c>
+      <c r="J9" s="9">
+        <v>10.84</v>
+      </c>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2">
+        <v>80393</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.62</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.38</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="9">
+        <v>92496</v>
+      </c>
+      <c r="H10" s="9">
+        <v>8.24</v>
+      </c>
+      <c r="I10" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="J10" s="9">
+        <v>4.08</v>
+      </c>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2">
+        <v>41929</v>
+      </c>
+      <c r="C11" s="2">
+        <v>13.21</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6.37</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.59</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="9">
+        <v>41929</v>
+      </c>
+      <c r="H11" s="9">
+        <v>13.21</v>
+      </c>
+      <c r="I11" s="9">
+        <v>6.37</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.59</v>
+      </c>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2">
+        <v>52253</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12.41</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="9">
+        <v>52253</v>
+      </c>
+      <c r="H12" s="9">
+        <v>12.41</v>
+      </c>
+      <c r="I12" s="9">
+        <v>6</v>
+      </c>
+      <c r="J12" s="9">
+        <v>4.4400000000000004</v>
+      </c>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <v>69014</v>
+      </c>
+      <c r="C13" s="2">
+        <v>10.43</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3.56</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9">
+        <v>69014</v>
+      </c>
+      <c r="H13" s="9">
+        <v>10.43</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J13" s="9">
+        <v>3.56</v>
+      </c>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
@@ -5535,405 +6565,19 @@
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C13)</f>
-        <v>0</v>
+        <v>164.95000000000002</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="9">
         <f>SUM(H2:H13)</f>
-        <v>0</v>
+        <v>164.95000000000005</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FC2FBA-017B-4C34-B19F-488BCA852EC5}">
-  <dimension ref="A1:AD30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="3" customWidth="1"/>
-    <col min="4" max="5" width="16.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="22" style="9" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="9"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="2"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="7"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-    </row>
-    <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="7"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-    </row>
-    <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="7"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
-    </row>
-    <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="7"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-    </row>
-    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="7"/>
-      <c r="AA7" s="2"/>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-      <c r="AD7" s="2"/>
-    </row>
-    <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="7"/>
-      <c r="AA8" s="2"/>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
-      <c r="AD8" s="2"/>
-    </row>
-    <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="7"/>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2"/>
-    </row>
-    <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="7"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-    </row>
-    <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="7"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2"/>
-    </row>
-    <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="7"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2"/>
-    </row>
-    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="7"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-    </row>
-    <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="5">
-        <f>SUM(C2:C13)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="9">
-        <f>SUM(H2:H13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>5</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <v>6</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -6495,7 +7139,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -6503,7 +7147,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -6542,7 +7186,7 @@
   <dimension ref="A1:AD16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6603,156 +7247,432 @@
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="G2" s="3"/>
-      <c r="J2" s="9"/>
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2">
+        <v>83257</v>
+      </c>
+      <c r="C2" s="2">
+        <v>19.57</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-0.8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>9.61</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="9">
+        <v>83257</v>
+      </c>
+      <c r="H2" s="9">
+        <v>19.57</v>
+      </c>
+      <c r="I2" s="9">
+        <v>-0.8</v>
+      </c>
+      <c r="J2" s="9">
+        <v>9.61</v>
+      </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="G3" s="3"/>
-      <c r="J3" s="9"/>
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2">
+        <v>95799</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10.68</v>
+      </c>
+      <c r="D3" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="9">
+        <v>95799</v>
+      </c>
+      <c r="H3" s="9">
+        <v>10.68</v>
+      </c>
+      <c r="I3" s="9">
+        <v>8.4</v>
+      </c>
+      <c r="J3" s="9">
+        <v>3.22</v>
+      </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="G4" s="3"/>
-      <c r="J4" s="9"/>
+      <c r="A4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2">
+        <v>82453</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15.68</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6.49</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9">
+        <v>82453</v>
+      </c>
+      <c r="H4" s="9">
+        <v>15.68</v>
+      </c>
+      <c r="I4" s="9">
+        <v>2</v>
+      </c>
+      <c r="J4" s="9">
+        <v>6.49</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="G5" s="3"/>
-      <c r="J5" s="9"/>
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2">
+        <v>42500</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12.68</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5.01</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9">
+        <v>42500</v>
+      </c>
+      <c r="H5" s="9">
+        <v>12.68</v>
+      </c>
+      <c r="I5" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="J5" s="9">
+        <v>5.01</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="G6" s="3"/>
-      <c r="J6" s="9"/>
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2">
+        <v>90444</v>
+      </c>
+      <c r="C6" s="2">
+        <v>13.32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4.71</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="9">
+        <v>90444</v>
+      </c>
+      <c r="H6" s="9">
+        <v>13.32</v>
+      </c>
+      <c r="I6" s="9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J6" s="9">
+        <v>4.71</v>
+      </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="G7" s="3"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2">
+        <v>87863</v>
+      </c>
+      <c r="C7" s="2">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10.43</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>51772</v>
+      </c>
+      <c r="H7" s="9">
+        <v>11.37</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="9">
+        <v>3.42</v>
+      </c>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="G8" s="3"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2">
+        <v>92496</v>
+      </c>
+      <c r="C8" s="2">
+        <v>7.94</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="9">
+        <v>78548</v>
+      </c>
+      <c r="H8" s="9">
+        <v>7.17</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="J8" s="9">
+        <v>1.71</v>
+      </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="G9" s="3"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>51772</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11.37</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.42</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9">
+        <v>87863</v>
+      </c>
+      <c r="H9" s="9">
+        <v>17</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1.8</v>
+      </c>
+      <c r="J9" s="9">
+        <v>10.43</v>
+      </c>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="G10" s="3"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2">
+        <v>78548</v>
+      </c>
+      <c r="C10" s="2">
+        <v>7.17</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="9">
+        <v>92496</v>
+      </c>
+      <c r="H10" s="9">
+        <v>7.94</v>
+      </c>
+      <c r="I10" s="9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J10" s="9">
+        <v>4.0199999999999996</v>
+      </c>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="3"/>
-      <c r="J11" s="9"/>
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2">
+        <v>70800</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14.06</v>
+      </c>
+      <c r="D11" s="2">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="9">
+        <v>70800</v>
+      </c>
+      <c r="H11" s="9">
+        <v>14.06</v>
+      </c>
+      <c r="I11" s="9">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J11" s="9">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="G12" s="3"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="2">
+        <v>87225</v>
+      </c>
+      <c r="C12" s="2">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="D12" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="9">
+        <v>38515</v>
+      </c>
+      <c r="H12" s="9">
+        <v>6.43</v>
+      </c>
+      <c r="I12" s="9">
+        <v>5.7</v>
+      </c>
+      <c r="J12" s="9">
+        <v>2.19</v>
+      </c>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="H13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="A13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="2">
+        <v>38515</v>
+      </c>
+      <c r="C13" s="2">
+        <v>6.43</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.19</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="9">
+        <v>87225</v>
+      </c>
+      <c r="H13" s="9">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="I13" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J13" s="9">
+        <v>4.4400000000000004</v>
+      </c>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
@@ -6765,19 +7685,20 @@
       </c>
       <c r="C15" s="5">
         <f>SUM(C2:C13)</f>
-        <v>0</v>
+        <v>144.45000000000002</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="9">
         <f>SUM(H2:H13)</f>
-        <v>0</v>
+        <v>144.45000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="8"/>
+      <c r="G16" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -7047,7 +7968,7 @@
         <v>12.02</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" s="9">
         <v>50301</v>
@@ -7104,7 +8025,7 @@
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1">
         <v>50301</v>
@@ -7176,7 +8097,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1">
         <v>41929</v>
@@ -7191,7 +8112,7 @@
         <v>4.6100000000000003</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9">
         <v>41929</v>
@@ -7227,7 +8148,7 @@
         <v>5.14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G12" s="9">
         <v>51495</v>
@@ -7248,7 +8169,7 @@
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1">
         <v>51495</v>
@@ -8179,7 +9100,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="9">
         <v>80393</v>
@@ -8200,7 +9121,7 @@
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="10">
         <v>80393</v>
@@ -8709,7 +9630,7 @@
         <v>4.12</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="3">
         <v>80393</v>
@@ -8730,7 +9651,7 @@
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2">
         <v>80393</v>
@@ -9297,7 +10218,7 @@
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>80393</v>
@@ -9348,7 +10269,7 @@
         <v>2.04</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" s="9">
         <v>80393</v>
@@ -9369,7 +10290,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -9384,7 +10305,7 @@
         <v>4.62</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9">
         <v>41929</v>
@@ -9900,7 +10821,7 @@
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2">
         <v>80393</v>
@@ -9915,7 +10836,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="9">
         <v>80393</v>
@@ -10559,7 +11480,7 @@
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>41929</v>
@@ -10574,7 +11495,7 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="9">
         <v>41929</v>
@@ -10631,7 +11552,7 @@
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2">
         <v>91573</v>
@@ -10646,7 +11567,7 @@
         <v>2.84</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="9">
         <v>91573</v>

</xml_diff>